<commit_message>
Reordering columns for Survey 1
</commit_message>
<xml_diff>
--- a/Surveys-CollectedData/CollectedData.xlsx
+++ b/Surveys-CollectedData/CollectedData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emadpres/university/papers/on-progress/ReplicationPackage/Surveys-CollectedData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BD21ED4-64D3-9743-B666-A9AED9E9A20C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{125C6BF3-232E-E942-8C28-0A30499A753E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-9220" yWindow="-28340" windowWidth="25600" windowHeight="23340" xr2:uid="{0859A35A-104C-F746-9241-13A79C37788E}"/>
+    <workbookView xWindow="-9220" yWindow="-28340" windowWidth="44300" windowHeight="24700" xr2:uid="{0859A35A-104C-F746-9241-13A79C37788E}"/>
   </bookViews>
   <sheets>
     <sheet name="Survey1" sheetId="3" r:id="rId1"/>
@@ -10665,13 +10665,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2465DACA-5FE0-7449-811F-7FC16538AFBC}">
   <dimension ref="A1:LQ82"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="91" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="91" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="5" max="5" width="35.5" customWidth="1"/>
+    <col min="2" max="2" width="35.5" customWidth="1"/>
     <col min="6" max="6" width="110.83203125" customWidth="1"/>
     <col min="7" max="7" width="51.33203125" customWidth="1"/>
     <col min="8" max="8" width="72.1640625" customWidth="1"/>
@@ -10698,16 +10698,16 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>4</v>
-      </c>
-      <c r="E1" t="s">
-        <v>1</v>
       </c>
       <c r="F1" t="s">
         <v>1618</v>
@@ -11683,20 +11683,20 @@
       </c>
     </row>
     <row r="2" spans="1:329" s="4" customFormat="1" ht="290" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
+        <v>434</v>
+      </c>
+      <c r="C2" t="s">
         <v>435</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>436</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>437</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>434</v>
       </c>
       <c r="F2" s="8" t="s">
         <v>1942</v>
@@ -12676,16 +12676,16 @@
         <v>867</v>
       </c>
       <c r="B3" t="s">
+        <v>868</v>
+      </c>
+      <c r="C3" t="s">
         <v>869</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>870</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>871</v>
-      </c>
-      <c r="E3" t="s">
-        <v>868</v>
       </c>
       <c r="F3" t="s">
         <v>2256</v>
@@ -13996,16 +13996,16 @@
         <v>100</v>
       </c>
       <c r="B5" t="s">
+        <v>2580</v>
+      </c>
+      <c r="C5" t="s">
         <v>890</v>
       </c>
-      <c r="C5">
-        <v>-99</v>
-      </c>
-      <c r="D5" t="s">
+      <c r="D5">
+        <v>-99</v>
+      </c>
+      <c r="E5" t="s">
         <v>904</v>
-      </c>
-      <c r="E5" t="s">
-        <v>2580</v>
       </c>
       <c r="F5" t="s">
         <v>2581</v>
@@ -14103,16 +14103,16 @@
         <v>100</v>
       </c>
       <c r="B6" t="s">
+        <v>2593</v>
+      </c>
+      <c r="C6" t="s">
         <v>890</v>
       </c>
-      <c r="C6">
-        <v>-99</v>
-      </c>
-      <c r="D6" t="s">
+      <c r="D6">
+        <v>-99</v>
+      </c>
+      <c r="E6" t="s">
         <v>937</v>
-      </c>
-      <c r="E6" t="s">
-        <v>2593</v>
       </c>
       <c r="F6" t="s">
         <v>2594</v>
@@ -14210,16 +14210,16 @@
         <v>100</v>
       </c>
       <c r="B7" t="s">
+        <v>2603</v>
+      </c>
+      <c r="C7" t="s">
         <v>918</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>2602</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>920</v>
-      </c>
-      <c r="E7" t="s">
-        <v>2603</v>
       </c>
       <c r="F7" t="s">
         <v>2604</v>
@@ -14317,16 +14317,16 @@
         <v>100</v>
       </c>
       <c r="B8" t="s">
+        <v>2618</v>
+      </c>
+      <c r="C8" t="s">
         <v>890</v>
       </c>
-      <c r="C8">
-        <v>-99</v>
-      </c>
-      <c r="D8" t="s">
+      <c r="D8">
+        <v>-99</v>
+      </c>
+      <c r="E8" t="s">
         <v>937</v>
-      </c>
-      <c r="E8" t="s">
-        <v>2618</v>
       </c>
       <c r="F8" t="s">
         <v>2619</v>
@@ -14424,16 +14424,16 @@
         <v>100</v>
       </c>
       <c r="B9" t="s">
+        <v>2627</v>
+      </c>
+      <c r="C9" t="s">
         <v>949</v>
       </c>
-      <c r="C9">
-        <v>-99</v>
-      </c>
-      <c r="D9" t="s">
+      <c r="D9">
+        <v>-99</v>
+      </c>
+      <c r="E9" t="s">
         <v>937</v>
-      </c>
-      <c r="E9" t="s">
-        <v>2627</v>
       </c>
       <c r="F9" t="s">
         <v>2628</v>
@@ -14531,16 +14531,16 @@
         <v>100</v>
       </c>
       <c r="B10" t="s">
+        <v>2633</v>
+      </c>
+      <c r="C10" t="s">
         <v>890</v>
       </c>
-      <c r="C10">
-        <v>-99</v>
-      </c>
-      <c r="D10" t="s">
+      <c r="D10">
+        <v>-99</v>
+      </c>
+      <c r="E10" t="s">
         <v>920</v>
-      </c>
-      <c r="E10" t="s">
-        <v>2633</v>
       </c>
       <c r="F10" t="s">
         <v>2634</v>
@@ -14638,16 +14638,16 @@
         <v>100</v>
       </c>
       <c r="B11" t="s">
+        <v>2643</v>
+      </c>
+      <c r="C11" t="s">
         <v>890</v>
       </c>
-      <c r="C11">
-        <v>-99</v>
-      </c>
-      <c r="D11" t="s">
+      <c r="D11">
+        <v>-99</v>
+      </c>
+      <c r="E11" t="s">
         <v>920</v>
-      </c>
-      <c r="E11" t="s">
-        <v>2643</v>
       </c>
       <c r="F11" t="s">
         <v>2644</v>
@@ -14745,16 +14745,16 @@
         <v>100</v>
       </c>
       <c r="B12" t="s">
+        <v>2651</v>
+      </c>
+      <c r="C12" t="s">
         <v>890</v>
       </c>
-      <c r="C12">
-        <v>-99</v>
-      </c>
-      <c r="D12" t="s">
+      <c r="D12">
+        <v>-99</v>
+      </c>
+      <c r="E12" t="s">
         <v>891</v>
-      </c>
-      <c r="E12" t="s">
-        <v>2651</v>
       </c>
       <c r="F12" t="s">
         <v>2634</v>
@@ -14852,16 +14852,16 @@
         <v>100</v>
       </c>
       <c r="B13" t="s">
+        <v>2661</v>
+      </c>
+      <c r="C13" t="s">
         <v>918</v>
       </c>
-      <c r="C13" t="s">
+      <c r="D13" t="s">
         <v>2660</v>
       </c>
-      <c r="D13" t="s">
+      <c r="E13" t="s">
         <v>904</v>
-      </c>
-      <c r="E13" t="s">
-        <v>2661</v>
       </c>
       <c r="F13" t="s">
         <v>2662</v>
@@ -14959,16 +14959,16 @@
         <v>100</v>
       </c>
       <c r="B14" t="s">
+        <v>2668</v>
+      </c>
+      <c r="C14" t="s">
         <v>890</v>
       </c>
-      <c r="C14">
-        <v>-99</v>
-      </c>
-      <c r="D14" t="s">
+      <c r="D14">
+        <v>-99</v>
+      </c>
+      <c r="E14" t="s">
         <v>937</v>
-      </c>
-      <c r="E14" t="s">
-        <v>2668</v>
       </c>
       <c r="F14" t="s">
         <v>2669</v>
@@ -15066,16 +15066,16 @@
         <v>100</v>
       </c>
       <c r="B15" t="s">
+        <v>2676</v>
+      </c>
+      <c r="C15" t="s">
         <v>890</v>
       </c>
-      <c r="C15">
-        <v>-99</v>
-      </c>
-      <c r="D15" t="s">
+      <c r="D15">
+        <v>-99</v>
+      </c>
+      <c r="E15" t="s">
         <v>920</v>
-      </c>
-      <c r="E15" t="s">
-        <v>2676</v>
       </c>
       <c r="F15" t="s">
         <v>2677</v>
@@ -15173,16 +15173,16 @@
         <v>100</v>
       </c>
       <c r="B16" t="s">
+        <v>2681</v>
+      </c>
+      <c r="C16" t="s">
         <v>977</v>
       </c>
-      <c r="C16">
-        <v>-99</v>
-      </c>
-      <c r="D16" t="s">
+      <c r="D16">
+        <v>-99</v>
+      </c>
+      <c r="E16" t="s">
         <v>937</v>
-      </c>
-      <c r="E16" t="s">
-        <v>2681</v>
       </c>
       <c r="F16" t="s">
         <v>2682</v>
@@ -15280,16 +15280,16 @@
         <v>100</v>
       </c>
       <c r="B17" t="s">
+        <v>2690</v>
+      </c>
+      <c r="C17" t="s">
         <v>890</v>
       </c>
-      <c r="C17">
-        <v>-99</v>
-      </c>
-      <c r="D17" t="s">
+      <c r="D17">
+        <v>-99</v>
+      </c>
+      <c r="E17" t="s">
         <v>904</v>
-      </c>
-      <c r="E17" t="s">
-        <v>2690</v>
       </c>
       <c r="F17" t="s">
         <v>2691</v>
@@ -15390,16 +15390,16 @@
         <v>100</v>
       </c>
       <c r="B18" t="s">
+        <v>2699</v>
+      </c>
+      <c r="C18" t="s">
         <v>918</v>
       </c>
-      <c r="C18" t="s">
+      <c r="D18" t="s">
         <v>2698</v>
       </c>
-      <c r="D18" t="s">
+      <c r="E18" t="s">
         <v>920</v>
-      </c>
-      <c r="E18" t="s">
-        <v>2699</v>
       </c>
       <c r="F18" t="s">
         <v>2700</v>
@@ -15497,16 +15497,16 @@
         <v>100</v>
       </c>
       <c r="B19" t="s">
+        <v>2709</v>
+      </c>
+      <c r="C19" t="s">
         <v>918</v>
       </c>
-      <c r="C19" t="s">
+      <c r="D19" t="s">
         <v>2708</v>
       </c>
-      <c r="D19" t="s">
+      <c r="E19" t="s">
         <v>920</v>
-      </c>
-      <c r="E19" t="s">
-        <v>2709</v>
       </c>
       <c r="F19" t="s">
         <v>2710</v>
@@ -15604,16 +15604,16 @@
         <v>100</v>
       </c>
       <c r="B20" t="s">
+        <v>2718</v>
+      </c>
+      <c r="C20" t="s">
         <v>918</v>
       </c>
-      <c r="C20" t="s">
+      <c r="D20" t="s">
         <v>2717</v>
       </c>
-      <c r="D20" t="s">
+      <c r="E20" t="s">
         <v>904</v>
-      </c>
-      <c r="E20" t="s">
-        <v>2718</v>
       </c>
       <c r="F20" t="s">
         <v>2719</v>
@@ -15717,16 +15717,16 @@
         <v>100</v>
       </c>
       <c r="B21" t="s">
+        <v>2732</v>
+      </c>
+      <c r="C21" t="s">
         <v>1022</v>
       </c>
-      <c r="C21">
-        <v>-99</v>
-      </c>
-      <c r="D21" t="s">
+      <c r="D21">
+        <v>-99</v>
+      </c>
+      <c r="E21" t="s">
         <v>904</v>
-      </c>
-      <c r="E21" t="s">
-        <v>2732</v>
       </c>
       <c r="F21" t="s">
         <v>2733</v>
@@ -15824,16 +15824,16 @@
         <v>100</v>
       </c>
       <c r="B22" t="s">
+        <v>2739</v>
+      </c>
+      <c r="C22" t="s">
         <v>918</v>
       </c>
-      <c r="C22" t="s">
+      <c r="D22" t="s">
         <v>2738</v>
       </c>
-      <c r="D22" t="s">
+      <c r="E22" t="s">
         <v>904</v>
-      </c>
-      <c r="E22" t="s">
-        <v>2739</v>
       </c>
       <c r="F22" t="s">
         <v>2740</v>
@@ -15931,16 +15931,16 @@
         <v>100</v>
       </c>
       <c r="B23" t="s">
+        <v>2746</v>
+      </c>
+      <c r="C23" t="s">
         <v>890</v>
       </c>
-      <c r="C23">
-        <v>-99</v>
-      </c>
-      <c r="D23" t="s">
+      <c r="D23">
+        <v>-99</v>
+      </c>
+      <c r="E23" t="s">
         <v>904</v>
-      </c>
-      <c r="E23" t="s">
-        <v>2746</v>
       </c>
       <c r="F23" t="s">
         <v>2747</v>
@@ -16038,16 +16038,16 @@
         <v>100</v>
       </c>
       <c r="B24" t="s">
+        <v>2752</v>
+      </c>
+      <c r="C24" t="s">
         <v>890</v>
       </c>
-      <c r="C24">
-        <v>-99</v>
-      </c>
-      <c r="D24" t="s">
+      <c r="D24">
+        <v>-99</v>
+      </c>
+      <c r="E24" t="s">
         <v>904</v>
-      </c>
-      <c r="E24" t="s">
-        <v>2752</v>
       </c>
       <c r="F24" t="s">
         <v>2753</v>
@@ -16148,16 +16148,16 @@
         <v>100</v>
       </c>
       <c r="B25" t="s">
+        <v>2761</v>
+      </c>
+      <c r="C25" t="s">
         <v>890</v>
       </c>
-      <c r="C25">
-        <v>-99</v>
-      </c>
-      <c r="D25" t="s">
+      <c r="D25">
+        <v>-99</v>
+      </c>
+      <c r="E25" t="s">
         <v>920</v>
-      </c>
-      <c r="E25" t="s">
-        <v>2761</v>
       </c>
       <c r="F25" t="s">
         <v>2762</v>
@@ -16255,16 +16255,16 @@
         <v>100</v>
       </c>
       <c r="B26" t="s">
+        <v>2769</v>
+      </c>
+      <c r="C26" t="s">
         <v>918</v>
       </c>
-      <c r="C26" t="s">
+      <c r="D26" t="s">
         <v>1320</v>
       </c>
-      <c r="D26" t="s">
+      <c r="E26" t="s">
         <v>937</v>
-      </c>
-      <c r="E26" t="s">
-        <v>2769</v>
       </c>
       <c r="F26" t="s">
         <v>2770</v>
@@ -16374,16 +16374,16 @@
         <v>100</v>
       </c>
       <c r="B27" t="s">
+        <v>2786</v>
+      </c>
+      <c r="C27" t="s">
         <v>890</v>
       </c>
-      <c r="C27">
-        <v>-99</v>
-      </c>
-      <c r="D27" t="s">
+      <c r="D27">
+        <v>-99</v>
+      </c>
+      <c r="E27" t="s">
         <v>920</v>
-      </c>
-      <c r="E27" t="s">
-        <v>2786</v>
       </c>
       <c r="F27" t="s">
         <v>2787</v>
@@ -16484,16 +16484,16 @@
         <v>100</v>
       </c>
       <c r="B28" t="s">
+        <v>2793</v>
+      </c>
+      <c r="C28" t="s">
         <v>977</v>
       </c>
-      <c r="C28">
-        <v>-99</v>
-      </c>
-      <c r="D28" t="s">
+      <c r="D28">
+        <v>-99</v>
+      </c>
+      <c r="E28" t="s">
         <v>937</v>
-      </c>
-      <c r="E28" t="s">
-        <v>2793</v>
       </c>
       <c r="F28" t="s">
         <v>2794</v>
@@ -16591,16 +16591,16 @@
         <v>100</v>
       </c>
       <c r="B29" t="s">
+        <v>2797</v>
+      </c>
+      <c r="C29" t="s">
         <v>890</v>
       </c>
-      <c r="C29">
-        <v>-99</v>
-      </c>
-      <c r="D29" t="s">
+      <c r="D29">
+        <v>-99</v>
+      </c>
+      <c r="E29" t="s">
         <v>891</v>
-      </c>
-      <c r="E29" t="s">
-        <v>2797</v>
       </c>
       <c r="F29" t="s">
         <v>2798</v>
@@ -16698,16 +16698,16 @@
         <v>100</v>
       </c>
       <c r="B30" t="s">
+        <v>2803</v>
+      </c>
+      <c r="C30" t="s">
         <v>918</v>
       </c>
-      <c r="C30" t="s">
+      <c r="D30" t="s">
         <v>2802</v>
       </c>
-      <c r="D30" t="s">
+      <c r="E30" t="s">
         <v>920</v>
-      </c>
-      <c r="E30" t="s">
-        <v>2803</v>
       </c>
       <c r="F30" t="s">
         <v>2804</v>
@@ -16805,16 +16805,16 @@
         <v>100</v>
       </c>
       <c r="B31" t="s">
+        <v>2810</v>
+      </c>
+      <c r="C31" t="s">
         <v>949</v>
       </c>
-      <c r="C31">
-        <v>-99</v>
-      </c>
-      <c r="D31" t="s">
+      <c r="D31">
+        <v>-99</v>
+      </c>
+      <c r="E31" t="s">
         <v>920</v>
-      </c>
-      <c r="E31" t="s">
-        <v>2810</v>
       </c>
       <c r="F31" t="s">
         <v>2811</v>
@@ -16912,16 +16912,16 @@
         <v>100</v>
       </c>
       <c r="B32" t="s">
+        <v>2817</v>
+      </c>
+      <c r="C32" t="s">
         <v>890</v>
       </c>
-      <c r="C32">
-        <v>-99</v>
-      </c>
-      <c r="D32" t="s">
+      <c r="D32">
+        <v>-99</v>
+      </c>
+      <c r="E32" t="s">
         <v>920</v>
-      </c>
-      <c r="E32" t="s">
-        <v>2817</v>
       </c>
       <c r="F32" t="s">
         <v>2818</v>
@@ -17022,16 +17022,16 @@
         <v>100</v>
       </c>
       <c r="B33" t="s">
+        <v>2828</v>
+      </c>
+      <c r="C33" t="s">
         <v>890</v>
       </c>
-      <c r="C33">
-        <v>-99</v>
-      </c>
-      <c r="D33" t="s">
+      <c r="D33">
+        <v>-99</v>
+      </c>
+      <c r="E33" t="s">
         <v>920</v>
-      </c>
-      <c r="E33" t="s">
-        <v>2828</v>
       </c>
       <c r="F33" t="s">
         <v>2829</v>
@@ -17132,16 +17132,16 @@
         <v>100</v>
       </c>
       <c r="B34" t="s">
+        <v>2839</v>
+      </c>
+      <c r="C34" t="s">
         <v>1022</v>
       </c>
-      <c r="C34">
-        <v>-99</v>
-      </c>
-      <c r="D34" t="s">
+      <c r="D34">
+        <v>-99</v>
+      </c>
+      <c r="E34" t="s">
         <v>937</v>
-      </c>
-      <c r="E34" t="s">
-        <v>2839</v>
       </c>
       <c r="F34" t="s">
         <v>2840</v>
@@ -17239,16 +17239,16 @@
         <v>100</v>
       </c>
       <c r="B35" t="s">
+        <v>2850</v>
+      </c>
+      <c r="C35" t="s">
         <v>1022</v>
       </c>
-      <c r="C35">
-        <v>-99</v>
-      </c>
-      <c r="D35" t="s">
+      <c r="D35">
+        <v>-99</v>
+      </c>
+      <c r="E35" t="s">
         <v>937</v>
-      </c>
-      <c r="E35" t="s">
-        <v>2850</v>
       </c>
       <c r="F35" t="s">
         <v>2851</v>
@@ -17346,16 +17346,16 @@
         <v>100</v>
       </c>
       <c r="B36" t="s">
+        <v>2858</v>
+      </c>
+      <c r="C36" t="s">
         <v>890</v>
       </c>
-      <c r="C36">
-        <v>-99</v>
-      </c>
-      <c r="D36" t="s">
+      <c r="D36">
+        <v>-99</v>
+      </c>
+      <c r="E36" t="s">
         <v>904</v>
-      </c>
-      <c r="E36" t="s">
-        <v>2858</v>
       </c>
       <c r="F36" t="s">
         <v>2859</v>
@@ -17462,16 +17462,16 @@
         <v>100</v>
       </c>
       <c r="B37" t="s">
+        <v>2874</v>
+      </c>
+      <c r="C37" t="s">
         <v>918</v>
       </c>
-      <c r="C37" t="s">
+      <c r="D37" t="s">
         <v>2873</v>
       </c>
-      <c r="D37" t="s">
+      <c r="E37" t="s">
         <v>891</v>
-      </c>
-      <c r="E37" t="s">
-        <v>2874</v>
       </c>
       <c r="F37" t="s">
         <v>2875</v>
@@ -17569,16 +17569,16 @@
         <v>100</v>
       </c>
       <c r="B38" t="s">
+        <v>2879</v>
+      </c>
+      <c r="C38" t="s">
         <v>918</v>
       </c>
-      <c r="C38" t="s">
+      <c r="D38" t="s">
         <v>2878</v>
       </c>
-      <c r="D38" t="s">
+      <c r="E38" t="s">
         <v>937</v>
-      </c>
-      <c r="E38" t="s">
-        <v>2879</v>
       </c>
       <c r="F38" t="s">
         <v>2880</v>
@@ -17676,16 +17676,16 @@
         <v>100</v>
       </c>
       <c r="B39" t="s">
+        <v>2884</v>
+      </c>
+      <c r="C39" t="s">
         <v>949</v>
       </c>
-      <c r="C39">
-        <v>-99</v>
-      </c>
-      <c r="D39" t="s">
+      <c r="D39">
+        <v>-99</v>
+      </c>
+      <c r="E39" t="s">
         <v>920</v>
-      </c>
-      <c r="E39" t="s">
-        <v>2884</v>
       </c>
       <c r="F39" t="s">
         <v>2885</v>
@@ -17783,16 +17783,16 @@
         <v>100</v>
       </c>
       <c r="B40" t="s">
+        <v>2891</v>
+      </c>
+      <c r="C40" t="s">
         <v>918</v>
       </c>
-      <c r="C40" t="s">
+      <c r="D40" t="s">
         <v>2890</v>
       </c>
-      <c r="D40" t="s">
+      <c r="E40" t="s">
         <v>920</v>
-      </c>
-      <c r="E40" t="s">
-        <v>2891</v>
       </c>
       <c r="F40" t="s">
         <v>2892</v>
@@ -17890,16 +17890,16 @@
         <v>100</v>
       </c>
       <c r="B41" t="s">
+        <v>2899</v>
+      </c>
+      <c r="C41" t="s">
         <v>918</v>
       </c>
-      <c r="C41" t="s">
+      <c r="D41" t="s">
         <v>2898</v>
       </c>
-      <c r="D41" t="s">
+      <c r="E41" t="s">
         <v>920</v>
-      </c>
-      <c r="E41" t="s">
-        <v>2899</v>
       </c>
       <c r="F41" t="s">
         <v>2900</v>
@@ -18012,16 +18012,16 @@
         <v>100</v>
       </c>
       <c r="B42" t="s">
+        <v>2917</v>
+      </c>
+      <c r="C42" t="s">
         <v>890</v>
       </c>
-      <c r="C42">
-        <v>-99</v>
-      </c>
-      <c r="D42" t="s">
+      <c r="D42">
+        <v>-99</v>
+      </c>
+      <c r="E42" t="s">
         <v>891</v>
-      </c>
-      <c r="E42" t="s">
-        <v>2917</v>
       </c>
       <c r="F42" t="s">
         <v>2918</v>
@@ -18119,16 +18119,16 @@
         <v>100</v>
       </c>
       <c r="B43" t="s">
+        <v>2922</v>
+      </c>
+      <c r="C43" t="s">
         <v>949</v>
       </c>
-      <c r="C43">
-        <v>-99</v>
-      </c>
-      <c r="D43" t="s">
+      <c r="D43">
+        <v>-99</v>
+      </c>
+      <c r="E43" t="s">
         <v>937</v>
-      </c>
-      <c r="E43" t="s">
-        <v>2922</v>
       </c>
       <c r="F43" t="s">
         <v>2923</v>
@@ -18229,16 +18229,16 @@
         <v>100</v>
       </c>
       <c r="B44" t="s">
+        <v>2929</v>
+      </c>
+      <c r="C44" t="s">
         <v>949</v>
       </c>
-      <c r="C44">
-        <v>-99</v>
-      </c>
-      <c r="D44" t="s">
+      <c r="D44">
+        <v>-99</v>
+      </c>
+      <c r="E44" t="s">
         <v>937</v>
-      </c>
-      <c r="E44" t="s">
-        <v>2929</v>
       </c>
       <c r="F44" t="s">
         <v>2930</v>
@@ -18336,16 +18336,16 @@
         <v>100</v>
       </c>
       <c r="B45" t="s">
+        <v>2934</v>
+      </c>
+      <c r="C45" t="s">
         <v>890</v>
       </c>
-      <c r="C45">
-        <v>-99</v>
-      </c>
-      <c r="D45" t="s">
+      <c r="D45">
+        <v>-99</v>
+      </c>
+      <c r="E45" t="s">
         <v>937</v>
-      </c>
-      <c r="E45" t="s">
-        <v>2934</v>
       </c>
       <c r="F45" t="s">
         <v>2935</v>
@@ -18443,16 +18443,16 @@
         <v>100</v>
       </c>
       <c r="B46" t="s">
+        <v>2939</v>
+      </c>
+      <c r="C46" t="s">
         <v>1022</v>
       </c>
-      <c r="C46">
-        <v>-99</v>
-      </c>
-      <c r="D46" t="s">
+      <c r="D46">
+        <v>-99</v>
+      </c>
+      <c r="E46" t="s">
         <v>920</v>
-      </c>
-      <c r="E46" t="s">
-        <v>2939</v>
       </c>
       <c r="F46" t="s">
         <v>2940</v>
@@ -18550,16 +18550,16 @@
         <v>100</v>
       </c>
       <c r="B47" t="s">
+        <v>2946</v>
+      </c>
+      <c r="C47" t="s">
         <v>949</v>
       </c>
-      <c r="C47">
-        <v>-99</v>
-      </c>
-      <c r="D47" t="s">
+      <c r="D47">
+        <v>-99</v>
+      </c>
+      <c r="E47" t="s">
         <v>937</v>
-      </c>
-      <c r="E47" t="s">
-        <v>2946</v>
       </c>
       <c r="F47" t="s">
         <v>2947</v>
@@ -18657,16 +18657,16 @@
         <v>100</v>
       </c>
       <c r="B48" t="s">
+        <v>2950</v>
+      </c>
+      <c r="C48" t="s">
         <v>890</v>
       </c>
-      <c r="C48">
-        <v>-99</v>
-      </c>
-      <c r="D48" t="s">
+      <c r="D48">
+        <v>-99</v>
+      </c>
+      <c r="E48" t="s">
         <v>904</v>
-      </c>
-      <c r="E48" t="s">
-        <v>2950</v>
       </c>
       <c r="F48" t="s">
         <v>2951</v>
@@ -18764,16 +18764,16 @@
         <v>100</v>
       </c>
       <c r="B49" t="s">
+        <v>2956</v>
+      </c>
+      <c r="C49" t="s">
         <v>918</v>
       </c>
-      <c r="C49" t="s">
+      <c r="D49" t="s">
         <v>2955</v>
       </c>
-      <c r="D49" t="s">
+      <c r="E49" t="s">
         <v>920</v>
-      </c>
-      <c r="E49" t="s">
-        <v>2956</v>
       </c>
       <c r="F49" t="s">
         <v>2957</v>
@@ -18874,16 +18874,16 @@
         <v>100</v>
       </c>
       <c r="B50" t="s">
+        <v>2963</v>
+      </c>
+      <c r="C50" t="s">
         <v>890</v>
       </c>
-      <c r="C50">
-        <v>-99</v>
-      </c>
-      <c r="D50" t="s">
+      <c r="D50">
+        <v>-99</v>
+      </c>
+      <c r="E50" t="s">
         <v>937</v>
-      </c>
-      <c r="E50" t="s">
-        <v>2963</v>
       </c>
       <c r="F50" t="s">
         <v>2964</v>
@@ -18987,16 +18987,16 @@
         <v>100</v>
       </c>
       <c r="B51" t="s">
+        <v>2972</v>
+      </c>
+      <c r="C51" t="s">
         <v>949</v>
       </c>
-      <c r="C51">
-        <v>-99</v>
-      </c>
-      <c r="D51" t="s">
+      <c r="D51">
+        <v>-99</v>
+      </c>
+      <c r="E51" t="s">
         <v>920</v>
-      </c>
-      <c r="E51" t="s">
-        <v>2972</v>
       </c>
       <c r="F51" t="s">
         <v>2973</v>
@@ -19094,16 +19094,16 @@
         <v>100</v>
       </c>
       <c r="B52" t="s">
+        <v>2979</v>
+      </c>
+      <c r="C52" t="s">
         <v>890</v>
       </c>
-      <c r="C52">
-        <v>-99</v>
-      </c>
-      <c r="D52" t="s">
+      <c r="D52">
+        <v>-99</v>
+      </c>
+      <c r="E52" t="s">
         <v>891</v>
-      </c>
-      <c r="E52" t="s">
-        <v>2979</v>
       </c>
       <c r="F52" t="s">
         <v>2980</v>
@@ -19204,16 +19204,16 @@
         <v>100</v>
       </c>
       <c r="B53" t="s">
+        <v>2992</v>
+      </c>
+      <c r="C53" t="s">
         <v>1022</v>
       </c>
-      <c r="C53">
-        <v>-99</v>
-      </c>
-      <c r="D53" t="s">
+      <c r="D53">
+        <v>-99</v>
+      </c>
+      <c r="E53" t="s">
         <v>920</v>
-      </c>
-      <c r="E53" t="s">
-        <v>2992</v>
       </c>
       <c r="F53" t="s">
         <v>2993</v>
@@ -19314,16 +19314,16 @@
         <v>100</v>
       </c>
       <c r="B54" t="s">
+        <v>2999</v>
+      </c>
+      <c r="C54" t="s">
         <v>890</v>
       </c>
-      <c r="C54">
-        <v>-99</v>
-      </c>
-      <c r="D54" t="s">
+      <c r="D54">
+        <v>-99</v>
+      </c>
+      <c r="E54" t="s">
         <v>920</v>
-      </c>
-      <c r="E54" t="s">
-        <v>2999</v>
       </c>
       <c r="F54" t="s">
         <v>3000</v>
@@ -19421,16 +19421,16 @@
         <v>100</v>
       </c>
       <c r="B55" t="s">
+        <v>3004</v>
+      </c>
+      <c r="C55" t="s">
         <v>890</v>
       </c>
-      <c r="C55">
-        <v>-99</v>
-      </c>
-      <c r="D55" t="s">
+      <c r="D55">
+        <v>-99</v>
+      </c>
+      <c r="E55" t="s">
         <v>920</v>
-      </c>
-      <c r="E55" t="s">
-        <v>3004</v>
       </c>
       <c r="F55" t="s">
         <v>3005</v>
@@ -19531,16 +19531,16 @@
         <v>100</v>
       </c>
       <c r="B56" t="s">
+        <v>3017</v>
+      </c>
+      <c r="C56" t="s">
         <v>949</v>
       </c>
-      <c r="C56">
-        <v>-99</v>
-      </c>
-      <c r="D56" t="s">
+      <c r="D56">
+        <v>-99</v>
+      </c>
+      <c r="E56" t="s">
         <v>920</v>
-      </c>
-      <c r="E56" t="s">
-        <v>3017</v>
       </c>
       <c r="F56" t="s">
         <v>3018</v>
@@ -19638,16 +19638,16 @@
         <v>100</v>
       </c>
       <c r="B57" t="s">
+        <v>3023</v>
+      </c>
+      <c r="C57" t="s">
         <v>890</v>
       </c>
-      <c r="C57">
-        <v>-99</v>
-      </c>
-      <c r="D57" t="s">
+      <c r="D57">
+        <v>-99</v>
+      </c>
+      <c r="E57" t="s">
         <v>920</v>
-      </c>
-      <c r="E57" t="s">
-        <v>3023</v>
       </c>
       <c r="F57" t="s">
         <v>2799</v>
@@ -19745,16 +19745,16 @@
         <v>100</v>
       </c>
       <c r="B58" t="s">
+        <v>3025</v>
+      </c>
+      <c r="C58" t="s">
         <v>890</v>
       </c>
-      <c r="C58">
-        <v>-99</v>
-      </c>
-      <c r="D58" t="s">
+      <c r="D58">
+        <v>-99</v>
+      </c>
+      <c r="E58" t="s">
         <v>937</v>
-      </c>
-      <c r="E58" t="s">
-        <v>3025</v>
       </c>
       <c r="F58" t="s">
         <v>3026</v>
@@ -19855,16 +19855,16 @@
         <v>100</v>
       </c>
       <c r="B59" t="s">
+        <v>3033</v>
+      </c>
+      <c r="C59" t="s">
         <v>890</v>
       </c>
-      <c r="C59">
-        <v>-99</v>
-      </c>
-      <c r="D59" t="s">
+      <c r="D59">
+        <v>-99</v>
+      </c>
+      <c r="E59" t="s">
         <v>920</v>
-      </c>
-      <c r="E59" t="s">
-        <v>3033</v>
       </c>
       <c r="F59" t="s">
         <v>3034</v>
@@ -19962,16 +19962,16 @@
         <v>100</v>
       </c>
       <c r="B60" t="s">
+        <v>3043</v>
+      </c>
+      <c r="C60" t="s">
         <v>918</v>
       </c>
-      <c r="C60" t="s">
+      <c r="D60" t="s">
         <v>3042</v>
       </c>
-      <c r="D60" t="s">
+      <c r="E60" t="s">
         <v>937</v>
-      </c>
-      <c r="E60" t="s">
-        <v>3043</v>
       </c>
       <c r="F60" t="s">
         <v>3044</v>
@@ -20069,16 +20069,16 @@
         <v>100</v>
       </c>
       <c r="B61" t="s">
+        <v>3050</v>
+      </c>
+      <c r="C61" t="s">
         <v>1022</v>
       </c>
-      <c r="C61">
-        <v>-99</v>
-      </c>
-      <c r="D61" t="s">
+      <c r="D61">
+        <v>-99</v>
+      </c>
+      <c r="E61" t="s">
         <v>920</v>
-      </c>
-      <c r="E61" t="s">
-        <v>3050</v>
       </c>
       <c r="F61" t="s">
         <v>3051</v>
@@ -20179,16 +20179,16 @@
         <v>100</v>
       </c>
       <c r="B62" t="s">
+        <v>3055</v>
+      </c>
+      <c r="C62" t="s">
         <v>890</v>
       </c>
-      <c r="C62">
-        <v>-99</v>
-      </c>
-      <c r="D62" t="s">
+      <c r="D62">
+        <v>-99</v>
+      </c>
+      <c r="E62" t="s">
         <v>937</v>
-      </c>
-      <c r="E62" t="s">
-        <v>3055</v>
       </c>
       <c r="F62" t="s">
         <v>3056</v>
@@ -20286,16 +20286,16 @@
         <v>100</v>
       </c>
       <c r="B63" t="s">
+        <v>3060</v>
+      </c>
+      <c r="C63" t="s">
         <v>918</v>
       </c>
-      <c r="C63" t="s">
+      <c r="D63" t="s">
         <v>3059</v>
       </c>
-      <c r="D63" t="s">
+      <c r="E63" t="s">
         <v>920</v>
-      </c>
-      <c r="E63" t="s">
-        <v>3060</v>
       </c>
       <c r="F63" t="s">
         <v>3061</v>
@@ -20393,16 +20393,16 @@
         <v>100</v>
       </c>
       <c r="B64" t="s">
+        <v>3067</v>
+      </c>
+      <c r="C64" t="s">
         <v>890</v>
       </c>
-      <c r="C64">
-        <v>-99</v>
-      </c>
-      <c r="D64" t="s">
+      <c r="D64">
+        <v>-99</v>
+      </c>
+      <c r="E64" t="s">
         <v>904</v>
-      </c>
-      <c r="E64" t="s">
-        <v>3067</v>
       </c>
       <c r="F64" t="s">
         <v>3068</v>
@@ -20500,16 +20500,16 @@
         <v>100</v>
       </c>
       <c r="B65" t="s">
+        <v>3075</v>
+      </c>
+      <c r="C65" t="s">
         <v>949</v>
       </c>
-      <c r="C65">
-        <v>-99</v>
-      </c>
-      <c r="D65" t="s">
+      <c r="D65">
+        <v>-99</v>
+      </c>
+      <c r="E65" t="s">
         <v>920</v>
-      </c>
-      <c r="E65" t="s">
-        <v>3075</v>
       </c>
       <c r="F65" t="s">
         <v>3076</v>
@@ -20607,16 +20607,16 @@
         <v>100</v>
       </c>
       <c r="B66" t="s">
+        <v>3079</v>
+      </c>
+      <c r="C66" t="s">
         <v>890</v>
       </c>
-      <c r="C66">
-        <v>-99</v>
-      </c>
-      <c r="D66" t="s">
+      <c r="D66">
+        <v>-99</v>
+      </c>
+      <c r="E66" t="s">
         <v>891</v>
-      </c>
-      <c r="E66" t="s">
-        <v>3079</v>
       </c>
       <c r="F66" t="s">
         <v>3080</v>
@@ -20714,16 +20714,16 @@
         <v>100</v>
       </c>
       <c r="B67" t="s">
+        <v>3085</v>
+      </c>
+      <c r="C67" t="s">
         <v>1022</v>
       </c>
-      <c r="C67">
-        <v>-99</v>
-      </c>
-      <c r="D67" t="s">
+      <c r="D67">
+        <v>-99</v>
+      </c>
+      <c r="E67" t="s">
         <v>920</v>
-      </c>
-      <c r="E67" t="s">
-        <v>3085</v>
       </c>
       <c r="F67" t="s">
         <v>3086</v>
@@ -20821,16 +20821,16 @@
         <v>100</v>
       </c>
       <c r="B68" t="s">
+        <v>3092</v>
+      </c>
+      <c r="C68" t="s">
         <v>949</v>
       </c>
-      <c r="C68">
-        <v>-99</v>
-      </c>
-      <c r="D68" t="s">
+      <c r="D68">
+        <v>-99</v>
+      </c>
+      <c r="E68" t="s">
         <v>920</v>
-      </c>
-      <c r="E68" t="s">
-        <v>3092</v>
       </c>
       <c r="F68" t="s">
         <v>3093</v>
@@ -20928,16 +20928,16 @@
         <v>100</v>
       </c>
       <c r="B69" t="s">
+        <v>3098</v>
+      </c>
+      <c r="C69" t="s">
         <v>1022</v>
       </c>
-      <c r="C69">
-        <v>-99</v>
-      </c>
-      <c r="D69" t="s">
+      <c r="D69">
+        <v>-99</v>
+      </c>
+      <c r="E69" t="s">
         <v>920</v>
-      </c>
-      <c r="E69" t="s">
-        <v>3098</v>
       </c>
       <c r="F69" t="s">
         <v>3099</v>
@@ -21038,16 +21038,16 @@
         <v>100</v>
       </c>
       <c r="B70" t="s">
+        <v>3110</v>
+      </c>
+      <c r="C70" t="s">
         <v>977</v>
       </c>
-      <c r="C70">
-        <v>-99</v>
-      </c>
-      <c r="D70" t="s">
+      <c r="D70">
+        <v>-99</v>
+      </c>
+      <c r="E70" t="s">
         <v>920</v>
-      </c>
-      <c r="E70" t="s">
-        <v>3110</v>
       </c>
       <c r="F70" t="s">
         <v>3111</v>
@@ -21145,16 +21145,16 @@
         <v>100</v>
       </c>
       <c r="B71" t="s">
+        <v>3119</v>
+      </c>
+      <c r="C71" t="s">
         <v>918</v>
       </c>
-      <c r="C71" t="s">
+      <c r="D71" t="s">
         <v>3118</v>
       </c>
-      <c r="D71" t="s">
+      <c r="E71" t="s">
         <v>920</v>
-      </c>
-      <c r="E71" t="s">
-        <v>3119</v>
       </c>
       <c r="F71" t="s">
         <v>3120</v>
@@ -21255,16 +21255,16 @@
         <v>100</v>
       </c>
       <c r="B72" t="s">
+        <v>3130</v>
+      </c>
+      <c r="C72" t="s">
         <v>949</v>
       </c>
-      <c r="C72">
-        <v>-99</v>
-      </c>
-      <c r="D72" t="s">
+      <c r="D72">
+        <v>-99</v>
+      </c>
+      <c r="E72" t="s">
         <v>920</v>
-      </c>
-      <c r="E72" t="s">
-        <v>3130</v>
       </c>
       <c r="F72" t="s">
         <v>3131</v>
@@ -21362,16 +21362,16 @@
         <v>100</v>
       </c>
       <c r="B73" t="s">
+        <v>3138</v>
+      </c>
+      <c r="C73" t="s">
         <v>918</v>
       </c>
-      <c r="C73" t="s">
+      <c r="D73" t="s">
         <v>3137</v>
       </c>
-      <c r="D73" t="s">
+      <c r="E73" t="s">
         <v>920</v>
-      </c>
-      <c r="E73" t="s">
-        <v>3138</v>
       </c>
       <c r="F73" t="s">
         <v>3139</v>
@@ -21469,16 +21469,16 @@
         <v>100</v>
       </c>
       <c r="B74" t="s">
+        <v>3144</v>
+      </c>
+      <c r="C74" t="s">
         <v>949</v>
       </c>
-      <c r="C74">
-        <v>-99</v>
-      </c>
-      <c r="D74" t="s">
+      <c r="D74">
+        <v>-99</v>
+      </c>
+      <c r="E74" t="s">
         <v>937</v>
-      </c>
-      <c r="E74" t="s">
-        <v>3144</v>
       </c>
       <c r="F74" t="s">
         <v>3145</v>
@@ -21576,16 +21576,16 @@
         <v>100</v>
       </c>
       <c r="B75" t="s">
+        <v>3146</v>
+      </c>
+      <c r="C75" t="s">
         <v>918</v>
       </c>
-      <c r="C75" t="s">
+      <c r="D75" t="s">
         <v>2898</v>
       </c>
-      <c r="D75" t="s">
+      <c r="E75" t="s">
         <v>920</v>
-      </c>
-      <c r="E75" t="s">
-        <v>3146</v>
       </c>
       <c r="F75" t="s">
         <v>3147</v>
@@ -21689,16 +21689,16 @@
         <v>100</v>
       </c>
       <c r="B76" t="s">
+        <v>3157</v>
+      </c>
+      <c r="C76" t="s">
         <v>890</v>
       </c>
-      <c r="C76">
-        <v>-99</v>
-      </c>
-      <c r="D76" t="s">
+      <c r="D76">
+        <v>-99</v>
+      </c>
+      <c r="E76" t="s">
         <v>891</v>
-      </c>
-      <c r="E76" t="s">
-        <v>3157</v>
       </c>
       <c r="F76" t="s">
         <v>3158</v>
@@ -21796,16 +21796,16 @@
         <v>100</v>
       </c>
       <c r="B77" t="s">
+        <v>3161</v>
+      </c>
+      <c r="C77" t="s">
         <v>1022</v>
       </c>
-      <c r="C77">
-        <v>-99</v>
-      </c>
-      <c r="D77" t="s">
+      <c r="D77">
+        <v>-99</v>
+      </c>
+      <c r="E77" t="s">
         <v>920</v>
-      </c>
-      <c r="E77" t="s">
-        <v>3161</v>
       </c>
       <c r="F77" t="s">
         <v>3162</v>
@@ -21906,16 +21906,16 @@
         <v>100</v>
       </c>
       <c r="B78" t="s">
+        <v>3173</v>
+      </c>
+      <c r="C78" t="s">
         <v>890</v>
       </c>
-      <c r="C78">
-        <v>-99</v>
-      </c>
-      <c r="D78" t="s">
+      <c r="D78">
+        <v>-99</v>
+      </c>
+      <c r="E78" t="s">
         <v>920</v>
-      </c>
-      <c r="E78" t="s">
-        <v>3173</v>
       </c>
       <c r="F78" t="s">
         <v>3174</v>
@@ -22013,16 +22013,16 @@
         <v>100</v>
       </c>
       <c r="B79" t="s">
+        <v>3176</v>
+      </c>
+      <c r="C79" t="s">
         <v>1022</v>
       </c>
-      <c r="C79">
-        <v>-99</v>
-      </c>
-      <c r="D79" t="s">
+      <c r="D79">
+        <v>-99</v>
+      </c>
+      <c r="E79" t="s">
         <v>920</v>
-      </c>
-      <c r="E79" t="s">
-        <v>3176</v>
       </c>
       <c r="F79" t="s">
         <v>3177</v>
@@ -22120,16 +22120,16 @@
         <v>100</v>
       </c>
       <c r="B80" t="s">
+        <v>3181</v>
+      </c>
+      <c r="C80" t="s">
         <v>1022</v>
       </c>
-      <c r="C80">
-        <v>-99</v>
-      </c>
-      <c r="D80" t="s">
+      <c r="D80">
+        <v>-99</v>
+      </c>
+      <c r="E80" t="s">
         <v>920</v>
-      </c>
-      <c r="E80" t="s">
-        <v>3181</v>
       </c>
       <c r="F80" t="s">
         <v>3182</v>
@@ -22227,16 +22227,16 @@
         <v>100</v>
       </c>
       <c r="B81" t="s">
+        <v>3188</v>
+      </c>
+      <c r="C81" t="s">
         <v>949</v>
       </c>
-      <c r="C81">
-        <v>-99</v>
-      </c>
-      <c r="D81" t="s">
+      <c r="D81">
+        <v>-99</v>
+      </c>
+      <c r="E81" t="s">
         <v>920</v>
-      </c>
-      <c r="E81" t="s">
-        <v>3188</v>
       </c>
       <c r="F81" t="s">
         <v>3189</v>
@@ -22334,16 +22334,16 @@
         <v>100</v>
       </c>
       <c r="B82" t="s">
+        <v>3195</v>
+      </c>
+      <c r="C82" t="s">
         <v>890</v>
       </c>
-      <c r="C82">
-        <v>-99</v>
-      </c>
-      <c r="D82" t="s">
+      <c r="D82">
+        <v>-99</v>
+      </c>
+      <c r="E82" t="s">
         <v>937</v>
-      </c>
-      <c r="E82" t="s">
-        <v>3195</v>
       </c>
       <c r="F82" t="s">
         <v>3196</v>

</xml_diff>